<commit_message>
Added metadata file separate from datasheet
Edits to datasheet
</commit_message>
<xml_diff>
--- a/Data/Arran Field course 2023 data entry.xlsx
+++ b/Data/Arran Field course 2023 data entry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessshortman/Desktop/EIA/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BAEC06-1BC1-6446-9B84-8BF379041EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64AAF2D-6E6F-DA4C-9359-02152651E7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3640" yWindow="500" windowWidth="25160" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3334,27 +3334,18 @@
     <t>Terrestrial invertebrate observation data from associated occurrences (terreestrial invertebrates)</t>
   </si>
   <si>
-    <t>Sampling events (aquatic invertebrates)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Data of freshwater invertebrate presence was performed using kick sampling and rock rubbing </t>
   </si>
   <si>
     <t xml:space="preserve">Event ID corresponds to the plot (N=north, S=south) and the location (stream or marsh) </t>
   </si>
   <si>
-    <t>Associated occurrences (freshwater invertebraets)</t>
-  </si>
-  <si>
     <t>Freshwater invertebrate observation data from associated occurrences (freshwater invertebrates)</t>
   </si>
   <si>
     <t>Organisms are identified to family level wherever possible, or to order when family level identifications were not possible</t>
   </si>
   <si>
-    <t xml:space="preserve">Wateter flow conditions have been recorded as event remarks </t>
-  </si>
-  <si>
     <t>Organisms are identified to species level wherever possible, but mostly to family level  where lower level identifications were not possible</t>
   </si>
   <si>
@@ -3427,9 +3418,6 @@
     <t>Data on species presence was obtained during overnight camera trap surveys in both plots</t>
   </si>
   <si>
-    <t>Camrea trap presences from sampling events (camera traps)</t>
-  </si>
-  <si>
     <t xml:space="preserve">The species has been recorded with taxonomic information </t>
   </si>
   <si>
@@ -3442,7 +3430,19 @@
     <t>The sampling event in which the sighting was made has been recorded and species have been identified</t>
   </si>
   <si>
-    <t>Any additonal behavioural or habitat information on the sightings has been recorded</t>
+    <t>Associated occurrences (freshwater invertebrates)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water flow conditions have been recorded as event remarks </t>
+  </si>
+  <si>
+    <t>Sampling events (freshwater invertebrates)</t>
+  </si>
+  <si>
+    <t>Camera trap presences from sampling events (camera traps)</t>
+  </si>
+  <si>
+    <t>Any additional behavioural or habitat information on the sightings has been recorded</t>
   </si>
 </sst>
 </file>
@@ -4021,7 +4021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89161C00-A720-9643-8A16-AA9F00578D29}">
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B66" zoomScale="164" workbookViewId="0">
       <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
@@ -4201,38 +4201,38 @@
     </row>
     <row r="38" spans="1:2">
       <c r="B38" s="45" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="45" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B40" s="45" t="s">
         <v>1092</v>
-      </c>
-      <c r="B40" s="45" t="s">
-        <v>1093</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="B41" s="45" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="B42" s="45" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="B43" s="45" t="s">
-        <v>1098</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="45" t="s">
-        <v>1095</v>
+        <v>1124</v>
       </c>
       <c r="B45" s="45" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -4247,99 +4247,99 @@
     </row>
     <row r="48" spans="1:2">
       <c r="B48" s="45" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="45" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="B50" s="45" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="B51" s="45" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="B52" s="45" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="45" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="B54" s="45" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="B55" s="45" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="B56" s="45" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="45" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="B59" s="45" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="B60" s="45" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="B61" s="45" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="45" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="B63" s="45" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="B64" s="45" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="B65" s="45" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="45" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="B67" s="45" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="B68" s="45" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="B69" s="45" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -4347,10 +4347,10 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="45" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="B71" s="45" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -4360,38 +4360,38 @@
     </row>
     <row r="73" spans="1:2">
       <c r="B73" s="45" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="45" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="B75" s="45" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="B76" s="45" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="B77" s="45" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="B78" s="45" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="45" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="B80" s="45" t="s">
-        <v>1123</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -4401,20 +4401,20 @@
     </row>
     <row r="82" spans="1:2">
       <c r="B82" s="45" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="45" t="s">
-        <v>1125</v>
+        <v>1121</v>
       </c>
       <c r="B84" s="45" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="B85" s="45" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="86" spans="1:2">

</xml_diff>